<commit_message>
raw result of each team in gurobi/result
</commit_message>
<xml_diff>
--- a/Schedule and Starter.xlsx
+++ b/Schedule and Starter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matty\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\OneDrive\桌面\作業研究\Final Project\CPBL_OR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C1864D-5171-4FFC-AE08-54A1A68E853C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0336EA6-67CC-4A93-BFF9-3160CE5D5D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6550" xr2:uid="{038D55BE-E0D3-45D2-A4E9-4E10C0F78274}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{038D55BE-E0D3-45D2-A4E9-4E10C0F78274}"/>
   </bookViews>
   <sheets>
     <sheet name="中信兄弟" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="樂天桃猿" sheetId="5" r:id="rId4"/>
     <sheet name="味全龍" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -452,7 +452,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -468,7 +468,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -766,7 +766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22A18C3-3DD1-47E4-A8BD-CAE677AC2A26}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>